<commit_message>
added addtional data elements
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcutts/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF555C62-DC68-5D49-95AC-966422752114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145281D1-6000-264B-A368-E5C8A0A6D572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62040" yWindow="4900" windowWidth="28500" windowHeight="18600" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62040" yWindow="4900" windowWidth="28500" windowHeight="18600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="420">
   <si>
     <t>Description</t>
   </si>
@@ -1272,13 +1272,31 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>Data_capture_software</t>
-  </si>
-  <si>
     <t>Data Capture Software</t>
   </si>
   <si>
     <t>Indentier of the data processing software and version</t>
+  </si>
+  <si>
+    <t>drilling_activity_note</t>
+  </si>
+  <si>
+    <t>Drilling Activity Note</t>
+  </si>
+  <si>
+    <t>current_drilling_state</t>
+  </si>
+  <si>
+    <t>Current Drilling State</t>
+  </si>
+  <si>
+    <t>Make notes of things while drilling MWD, or transitioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auger drilling, Mud rtotary, hollow stem, rock core. </t>
+  </si>
+  <si>
+    <t>data_capture_software</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1472,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1496,6 +1514,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1506,6 +1530,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1743,8 +1773,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H42" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:H42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H44" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:H44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="12">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2863,1,FALSE)),"Not used","")</calculatedColumnFormula>
@@ -1762,8 +1792,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D42" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D42" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D44" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D44" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C2">
     <sortCondition ref="C1:C2"/>
   </sortState>
@@ -2126,10 +2156,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3116,20 +3146,62 @@
         <v/>
       </c>
       <c r="B42" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="C42" s="16" t="s">
         <v>411</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="D42" s="16" t="s">
         <v>412</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="E42" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="22"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B43,AssociatedElements!B$2:B2904,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>413</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="C43" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="E43" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="20"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="22"/>
+    </row>
+    <row r="44" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B44,AssociatedElements!B$2:B2905,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="22"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -3162,11 +3234,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3792,17 +3864,47 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="str">
+      <c r="A42" s="24" t="str">
         <f>IF(ISNA(VLOOKUP(B42,Definitions!B$2:B$1847,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B42" s="16" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>235</v>
       </c>
       <c r="D42" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="str">
+        <f>IF(ISNA(VLOOKUP(B43,Definitions!B$2:B$1847,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D43" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="24" t="str">
+        <f>IF(ISNA(VLOOKUP(B44,Definitions!B$2:B$1847,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D44" t="s">
         <v>410</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update conditional element xpaths
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60228506-C300-4049-A5C6-1D726847807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73C60F1-14C3-7846-9860-E75BAC98ABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -1011,9 +1011,6 @@
     <t>calibration flag</t>
   </si>
   <si>
-    <t>//diggs:MWDResult/diggs:results/diggs:ResultSet/diggs:parameters/diggs:PropertyParameters/diggs:properties/diggs:Property/diggs:propertyClass</t>
-  </si>
-  <si>
     <t>The measured depth downhole reached by the drill bit; a positive number.</t>
   </si>
   <si>
@@ -1146,10 +1143,13 @@
     <t>Torque: The rotational force applied by the drill rig.</t>
   </si>
   <si>
-    <t>//diggs:MWDResult</t>
-  </si>
-  <si>
     <t>This dictionary contains the values for the propertyClass property of the diggs:Property object for the Measurement While Drilling measurement object (diggs:/MeasurementWhileDrilling).</t>
+  </si>
+  <si>
+    <t>//diggs:propertyClass</t>
+  </si>
+  <si>
+    <t>../../../../../../../../MWDResult</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1319,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1370,24 +1370,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1396,13 +1378,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1419,56 +1394,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1566,6 +1491,56 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1693,30 +1668,30 @@
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D32" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D32" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D32" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C2">
     <sortCondition ref="C1:C2"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2003,7 +1978,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2054,7 +2029,7 @@
         <v>303</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -2071,7 +2046,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -2125,8 +2100,8 @@
       <c r="C2" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>346</v>
+      <c r="D2" s="22" t="s">
+        <v>345</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>174</v>
@@ -2149,8 +2124,8 @@
       <c r="C3" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>351</v>
+      <c r="D3" s="22" t="s">
+        <v>350</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>1</v>
@@ -2168,13 +2143,13 @@
         <v/>
       </c>
       <c r="B4" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>336</v>
+      <c r="D4" s="23" t="s">
+        <v>335</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>1</v>
@@ -2196,7 +2171,7 @@
         <v>254</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>1</v>
@@ -2219,8 +2194,8 @@
       <c r="C6" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>354</v>
+      <c r="D6" s="22" t="s">
+        <v>353</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>1</v>
@@ -2244,7 +2219,7 @@
         <v>246</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>1</v>
@@ -2267,8 +2242,8 @@
       <c r="C8" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>347</v>
+      <c r="D8" s="22" t="s">
+        <v>346</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>1</v>
@@ -2291,8 +2266,8 @@
       <c r="C9" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="D9" s="28" t="s">
-        <v>348</v>
+      <c r="D9" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>1</v>
@@ -2315,8 +2290,8 @@
       <c r="C10" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="D10" s="28" t="s">
-        <v>349</v>
+      <c r="D10" s="22" t="s">
+        <v>348</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>1</v>
@@ -2339,8 +2314,8 @@
       <c r="C11" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>350</v>
+      <c r="D11" s="22" t="s">
+        <v>349</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>1</v>
@@ -2358,13 +2333,13 @@
         <v/>
       </c>
       <c r="B12" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>355</v>
+      <c r="D12" s="22" t="s">
+        <v>354</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>180</v>
@@ -2386,7 +2361,7 @@
         <v>248</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>1</v>
@@ -2409,8 +2384,8 @@
       <c r="C14" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>357</v>
+      <c r="D14" s="22" t="s">
+        <v>356</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>1</v>
@@ -2434,7 +2409,7 @@
         <v>247</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>1</v>
@@ -2457,8 +2432,8 @@
       <c r="C16" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>359</v>
+      <c r="D16" s="22" t="s">
+        <v>358</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>1</v>
@@ -2470,7 +2445,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2850,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2479,10 +2454,10 @@
         <v>262</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>1</v>
@@ -2494,7 +2469,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B2851,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2506,7 +2481,7 @@
         <v>241</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>1</v>
@@ -2518,7 +2493,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2856,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2529,8 +2504,8 @@
       <c r="C19" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="D19" s="28" t="s">
-        <v>325</v>
+      <c r="D19" s="22" t="s">
+        <v>324</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>1</v>
@@ -2542,7 +2517,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2855,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2553,8 +2528,8 @@
       <c r="C20" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>364</v>
+      <c r="D20" s="22" t="s">
+        <v>363</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>1</v>
@@ -2566,7 +2541,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2854,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2577,8 +2552,8 @@
       <c r="C21" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="D21" s="28" t="s">
-        <v>362</v>
+      <c r="D21" s="22" t="s">
+        <v>361</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>1</v>
@@ -2590,7 +2565,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2844,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2601,8 +2576,8 @@
       <c r="C22" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="D22" s="28" t="s">
-        <v>363</v>
+      <c r="D22" s="22" t="s">
+        <v>362</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>1</v>
@@ -2614,7 +2589,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2876,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2626,7 +2601,7 @@
         <v>253</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>1</v>
@@ -2638,19 +2613,19 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2845,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B24" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>326</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>327</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>1</v>
@@ -2662,19 +2637,19 @@
         <v>281</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2846,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B25" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="D25" s="22" t="s">
         <v>329</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>330</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>1</v>
@@ -2686,7 +2661,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2875,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2697,8 +2672,8 @@
       <c r="C26" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D26" s="28" t="s">
-        <v>365</v>
+      <c r="D26" s="22" t="s">
+        <v>364</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>1</v>
@@ -2710,7 +2685,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2721,8 +2696,8 @@
       <c r="C27" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="D27" s="28" t="s">
-        <v>366</v>
+      <c r="D27" s="22" t="s">
+        <v>365</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>1</v>
@@ -2734,7 +2709,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2880,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2745,8 +2720,8 @@
       <c r="C28" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="D28" s="28" t="s">
-        <v>367</v>
+      <c r="D28" s="22" t="s">
+        <v>366</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>174</v>
@@ -2756,7 +2731,7 @@
       </c>
       <c r="G28" s="19"/>
     </row>
-    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2767,8 +2742,8 @@
       <c r="C29" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="D29" s="30" t="s">
-        <v>368</v>
+      <c r="D29" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>1</v>
@@ -2780,19 +2755,19 @@
         <v>278</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2881,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B30" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>306</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>1</v>
@@ -2802,19 +2777,19 @@
       </c>
       <c r="G30" s="19"/>
     </row>
-    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2852,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B31" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="D31" s="31" t="s">
-        <v>341</v>
+      <c r="D31" s="22" t="s">
+        <v>340</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>1</v>
@@ -2826,28 +2801,27 @@
         <v>288</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="str">
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="D32" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="D32" s="31" t="s">
-        <v>345</v>
-      </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="27"/>
-      <c r="H32" s="26"/>
+      <c r="G32" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -2884,14 +2858,14 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="118.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="93" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2918,10 +2892,10 @@
         <v>255</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2933,10 +2907,10 @@
         <v>256</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2948,10 +2922,10 @@
         <v>257</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2963,10 +2937,10 @@
         <v>258</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2978,10 +2952,10 @@
         <v>259</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D6" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2993,10 +2967,10 @@
         <v>260</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D7" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3008,10 +2982,10 @@
         <v>261</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3023,10 +2997,10 @@
         <v>262</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3038,10 +3012,10 @@
         <v>263</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3053,10 +3027,10 @@
         <v>264</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D11" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3068,10 +3042,10 @@
         <v>265</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3083,10 +3057,10 @@
         <v>266</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3098,10 +3072,10 @@
         <v>267</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D14" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3113,10 +3087,10 @@
         <v>268</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D15" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3128,10 +3102,10 @@
         <v>269</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D16" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3143,10 +3117,10 @@
         <v>270</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D17" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3158,10 +3132,10 @@
         <v>271</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D18" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3173,10 +3147,10 @@
         <v>272</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D19" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3188,10 +3162,10 @@
         <v>273</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D20" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3203,10 +3177,10 @@
         <v>274</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D21" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3218,10 +3192,10 @@
         <v>275</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D22" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3233,10 +3207,10 @@
         <v>276</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D23" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3248,10 +3222,10 @@
         <v>304</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D24" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3260,13 +3234,13 @@
         <v/>
       </c>
       <c r="B25" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D25" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3278,10 +3252,10 @@
         <v>322</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D26" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3290,13 +3264,13 @@
         <v/>
       </c>
       <c r="B27" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D27" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3305,13 +3279,13 @@
         <v/>
       </c>
       <c r="B28" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D28" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3320,13 +3294,13 @@
         <v/>
       </c>
       <c r="B29" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D29" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3335,43 +3309,43 @@
         <v/>
       </c>
       <c r="B30" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D30" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B31" s="33" t="s">
+      <c r="D31" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="str">
+        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" s="3" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>343</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="D32" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add borehole and sounding codelist dictionaries
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9E4B62-FB3A-A642-BBC4-432798E8ACA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298C97F0-6270-7A4B-B438-FB6DA9F28F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -765,9 +765,6 @@
     <t>Injected fluid dynamic viscosity</t>
   </si>
   <si>
-    <t>Vibration</t>
-  </si>
-  <si>
     <t>Inclination</t>
   </si>
   <si>
@@ -1114,6 +1111,9 @@
   </si>
   <si>
     <t>This dictionary contains the values for the propertyClass property contained within the the Measurement While Drilling measurement object (diggs:/MeasurementWhileDrilling).</t>
+  </si>
+  <si>
+    <t>Vibration acceleration</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1984,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2029,13 +2029,13 @@
         <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -2052,8 +2052,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:B24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2101,13 +2101,13 @@
         <v/>
       </c>
       <c r="B2" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>174</v>
@@ -2122,13 +2122,13 @@
         <v/>
       </c>
       <c r="B3" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>1</v>
@@ -2143,13 +2143,13 @@
         <v/>
       </c>
       <c r="B4" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>235</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>1</v>
@@ -2164,13 +2164,13 @@
         <v/>
       </c>
       <c r="B5" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>1</v>
@@ -2186,13 +2186,13 @@
         <v/>
       </c>
       <c r="B6" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>301</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>347</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>302</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>1</v>
@@ -2207,13 +2207,13 @@
         <v/>
       </c>
       <c r="B7" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>1</v>
@@ -2228,13 +2228,13 @@
         <v/>
       </c>
       <c r="B8" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>238</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>1</v>
@@ -2249,13 +2249,13 @@
         <v/>
       </c>
       <c r="B9" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>239</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>1</v>
@@ -2270,13 +2270,13 @@
         <v/>
       </c>
       <c r="B10" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>237</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>1</v>
@@ -2291,13 +2291,13 @@
         <v/>
       </c>
       <c r="B11" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>240</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>1</v>
@@ -2312,13 +2312,13 @@
         <v/>
       </c>
       <c r="B12" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>306</v>
-      </c>
       <c r="D12" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>180</v>
@@ -2334,13 +2334,13 @@
         <v/>
       </c>
       <c r="B13" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" s="33" t="s">
         <v>355</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="D13" s="30" t="s">
         <v>356</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>357</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>1</v>
@@ -2357,13 +2357,13 @@
         <v/>
       </c>
       <c r="B14" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" s="33" t="s">
         <v>352</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="D14" s="27" t="s">
         <v>353</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>354</v>
       </c>
       <c r="E14" s="28" t="s">
         <v>1</v>
@@ -2380,13 +2380,13 @@
         <v/>
       </c>
       <c r="B15" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>1</v>
@@ -2401,13 +2401,13 @@
         <v/>
       </c>
       <c r="B16" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>1</v>
@@ -2422,13 +2422,13 @@
         <v/>
       </c>
       <c r="B17" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>1</v>
@@ -2443,13 +2443,13 @@
         <v/>
       </c>
       <c r="B18" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>1</v>
@@ -2464,13 +2464,13 @@
         <v/>
       </c>
       <c r="B19" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>1</v>
@@ -2485,13 +2485,13 @@
         <v/>
       </c>
       <c r="B20" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>241</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>1</v>
@@ -2506,13 +2506,13 @@
         <v/>
       </c>
       <c r="B21" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>1</v>
@@ -2527,13 +2527,13 @@
         <v/>
       </c>
       <c r="B22" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>1</v>
@@ -2548,13 +2548,13 @@
         <v/>
       </c>
       <c r="B23" s="26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E23" s="28" t="s">
         <v>1</v>
@@ -2571,13 +2571,13 @@
         <v/>
       </c>
       <c r="B24" s="26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C24" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="D24" s="27" t="s">
         <v>342</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>343</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>174</v>
@@ -2593,13 +2593,13 @@
         <v/>
       </c>
       <c r="B25" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>1</v>
@@ -2614,13 +2614,13 @@
         <v/>
       </c>
       <c r="B26" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>236</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>1</v>
@@ -2635,13 +2635,13 @@
         <v/>
       </c>
       <c r="B27" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>1</v>
@@ -2656,13 +2656,13 @@
         <v/>
       </c>
       <c r="B28" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>299</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>311</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>300</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>1</v>
@@ -2677,13 +2677,13 @@
         <v/>
       </c>
       <c r="B29" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>1</v>
@@ -2698,13 +2698,13 @@
         <v/>
       </c>
       <c r="B30" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>1</v>
@@ -2719,13 +2719,13 @@
         <v/>
       </c>
       <c r="B31" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>281</v>
-      </c>
       <c r="D31" s="22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>174</v>
@@ -2741,13 +2741,13 @@
         <v/>
       </c>
       <c r="B32" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>234</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>1</v>
@@ -2762,13 +2762,13 @@
         <v/>
       </c>
       <c r="B33" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>1</v>
@@ -2784,13 +2784,13 @@
         <v/>
       </c>
       <c r="B34" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>242</v>
+        <v>358</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>1</v>
@@ -2805,13 +2805,13 @@
         <v/>
       </c>
       <c r="B35" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="C35" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="D35" s="22" t="s">
         <v>315</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>316</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>1</v>
@@ -2826,13 +2826,13 @@
         <v/>
       </c>
       <c r="B36" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E36" s="17" t="s">
         <v>1</v>
@@ -2907,13 +2907,13 @@
         <v/>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" t="s">
         <v>340</v>
-      </c>
-      <c r="D2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2922,13 +2922,13 @@
         <v/>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D3" t="s">
         <v>340</v>
-      </c>
-      <c r="D3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2937,13 +2937,13 @@
         <v/>
       </c>
       <c r="B4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D4" t="s">
         <v>340</v>
-      </c>
-      <c r="D4" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2952,13 +2952,13 @@
         <v/>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D5" t="s">
         <v>340</v>
-      </c>
-      <c r="D5" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2967,13 +2967,13 @@
         <v/>
       </c>
       <c r="B6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D6" t="s">
         <v>340</v>
-      </c>
-      <c r="D6" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2982,13 +2982,13 @@
         <v/>
       </c>
       <c r="B7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D7" t="s">
         <v>340</v>
-      </c>
-      <c r="D7" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2997,13 +2997,13 @@
         <v/>
       </c>
       <c r="B8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D8" t="s">
         <v>340</v>
-      </c>
-      <c r="D8" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3012,13 +3012,13 @@
         <v/>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" t="s">
         <v>340</v>
-      </c>
-      <c r="D9" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3027,13 +3027,13 @@
         <v/>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D10" t="s">
         <v>340</v>
-      </c>
-      <c r="D10" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3042,13 +3042,13 @@
         <v/>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D11" t="s">
         <v>340</v>
-      </c>
-      <c r="D11" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3057,13 +3057,13 @@
         <v/>
       </c>
       <c r="B12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D12" t="s">
         <v>340</v>
-      </c>
-      <c r="D12" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3072,13 +3072,13 @@
         <v/>
       </c>
       <c r="B13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D13" t="s">
         <v>340</v>
-      </c>
-      <c r="D13" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3087,13 +3087,13 @@
         <v/>
       </c>
       <c r="B14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" t="s">
         <v>340</v>
-      </c>
-      <c r="D14" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3102,13 +3102,13 @@
         <v/>
       </c>
       <c r="B15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D15" t="s">
         <v>340</v>
-      </c>
-      <c r="D15" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3117,13 +3117,13 @@
         <v/>
       </c>
       <c r="B16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D16" t="s">
         <v>340</v>
-      </c>
-      <c r="D16" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3132,13 +3132,13 @@
         <v/>
       </c>
       <c r="B17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D17" t="s">
         <v>340</v>
-      </c>
-      <c r="D17" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3147,13 +3147,13 @@
         <v/>
       </c>
       <c r="B18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D18" t="s">
         <v>340</v>
-      </c>
-      <c r="D18" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3162,13 +3162,13 @@
         <v/>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D19" t="s">
         <v>340</v>
-      </c>
-      <c r="D19" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3177,13 +3177,13 @@
         <v/>
       </c>
       <c r="B20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" t="s">
         <v>340</v>
-      </c>
-      <c r="D20" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3192,13 +3192,13 @@
         <v/>
       </c>
       <c r="B21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D21" t="s">
         <v>340</v>
-      </c>
-      <c r="D21" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3207,13 +3207,13 @@
         <v/>
       </c>
       <c r="B22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D22" t="s">
         <v>340</v>
-      </c>
-      <c r="D22" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3222,13 +3222,13 @@
         <v/>
       </c>
       <c r="B23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D23" t="s">
         <v>340</v>
-      </c>
-      <c r="D23" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3237,13 +3237,13 @@
         <v/>
       </c>
       <c r="B24" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D24" t="s">
         <v>340</v>
-      </c>
-      <c r="D24" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3252,13 +3252,13 @@
         <v/>
       </c>
       <c r="B25" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" t="s">
         <v>340</v>
-      </c>
-      <c r="D25" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3267,13 +3267,13 @@
         <v/>
       </c>
       <c r="B26" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D26" t="s">
         <v>340</v>
-      </c>
-      <c r="D26" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3282,13 +3282,13 @@
         <v/>
       </c>
       <c r="B27" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D27" t="s">
         <v>340</v>
-      </c>
-      <c r="D27" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3297,13 +3297,13 @@
         <v/>
       </c>
       <c r="B28" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D28" t="s">
         <v>340</v>
-      </c>
-      <c r="D28" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3312,13 +3312,13 @@
         <v/>
       </c>
       <c r="B29" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D29" t="s">
         <v>340</v>
-      </c>
-      <c r="D29" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3327,13 +3327,13 @@
         <v/>
       </c>
       <c r="B30" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D30" t="s">
         <v>340</v>
-      </c>
-      <c r="D30" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3342,13 +3342,13 @@
         <v/>
       </c>
       <c r="B31" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D31" t="s">
         <v>340</v>
-      </c>
-      <c r="D31" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3357,13 +3357,13 @@
         <v/>
       </c>
       <c r="B32" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D32" t="s">
         <v>340</v>
-      </c>
-      <c r="D32" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3372,13 +3372,13 @@
         <v/>
       </c>
       <c r="B33" s="37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D33" t="s">
         <v>340</v>
-      </c>
-      <c r="D33" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3387,13 +3387,13 @@
         <v/>
       </c>
       <c r="B34" s="37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D34" t="s">
         <v>340</v>
-      </c>
-      <c r="D34" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3402,13 +3402,13 @@
         <v/>
       </c>
       <c r="B35" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D35" t="s">
         <v>340</v>
-      </c>
-      <c r="D35" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3417,13 +3417,13 @@
         <v/>
       </c>
       <c r="B36" s="37" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D36" t="s">
         <v>340</v>
-      </c>
-      <c r="D36" t="s">
-        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -4704,77 +4704,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update properties and mwd_properteis xlsx files
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298C97F0-6270-7A4B-B438-FB6DA9F28F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68099EB0-F227-224F-97BD-CED95541CCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="1140" windowWidth="38400" windowHeight="19860" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -1059,9 +1059,6 @@
     <t>//diggs:propertyClass</t>
   </si>
   <si>
-    <t>../../../../../../../../MWDResult</t>
-  </si>
-  <si>
     <t>New rod event</t>
   </si>
   <si>
@@ -1114,6 +1111,9 @@
   </si>
   <si>
     <t>Vibration acceleration</t>
+  </si>
+  <si>
+    <t>../../../../../../../../../procedure/diggs:MWDProcedure</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1288,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1348,42 +1348,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1400,56 +1369,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1547,6 +1466,56 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FFFFFFFF"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1674,30 +1643,30 @@
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D36" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D36" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D36" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C2">
     <sortCondition ref="C1:C2"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2035,7 +2004,7 @@
         <v>278</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -2052,8 +2021,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2104,7 +2073,7 @@
         <v>296</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>316</v>
@@ -2167,9 +2136,9 @@
         <v>302</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="D5" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>306</v>
       </c>
       <c r="E5" s="17" t="s">
@@ -2189,7 +2158,7 @@
         <v>300</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>301</v>
@@ -2212,7 +2181,7 @@
       <c r="C7" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="19" t="s">
         <v>324</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -2329,50 +2298,48 @@
       <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="str">
+      <c r="A13" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B2876,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="D13" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>356</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="29"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="str">
+      <c r="A14" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B2875,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="D14" s="22" t="s">
         <v>352</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>353</v>
-      </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="29"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="str">
@@ -2416,7 +2383,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B2866,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2437,7 +2404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B2853,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2448,7 +2415,7 @@
       <c r="C18" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="19" t="s">
         <v>329</v>
       </c>
       <c r="E18" s="17" t="s">
@@ -2458,7 +2425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2850,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2479,7 +2446,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2851,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2500,7 +2467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2856,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2521,7 +2488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2855,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2542,52 +2509,50 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="str">
+    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="19"/>
+    </row>
+    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="str">
+        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="C23" s="33" t="s">
-        <v>347</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>350</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="29"/>
-    </row>
-    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>349</v>
-      </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="D24" s="27" t="s">
-        <v>342</v>
-      </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="29"/>
-    </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2854,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2608,7 +2573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2844,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2629,7 +2594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2876,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2650,7 +2615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2845,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2671,12 +2636,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2875,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="15" t="s">
         <v>273</v>
       </c>
       <c r="C29" s="18" t="s">
@@ -2692,7 +2657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2703,7 +2668,7 @@
       <c r="C30" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="19" t="s">
         <v>336</v>
       </c>
       <c r="E30" s="17" t="s">
@@ -2713,7 +2678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2880,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2735,7 +2700,7 @@
       </c>
       <c r="G31" s="19"/>
     </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="str">
         <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2764,8 +2729,8 @@
       <c r="B33" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="C33" s="34" t="s">
-        <v>345</v>
+      <c r="C33" s="26" t="s">
+        <v>344</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>307</v>
@@ -2786,10 +2751,10 @@
       <c r="B34" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="C34" s="34" t="s">
-        <v>358</v>
-      </c>
-      <c r="D34" s="35" t="s">
+      <c r="C34" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>311</v>
       </c>
       <c r="E34" s="17" t="s">
@@ -2807,7 +2772,7 @@
       <c r="B35" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="26" t="s">
         <v>314</v>
       </c>
       <c r="D35" s="22" t="s">
@@ -2828,7 +2793,7 @@
       <c r="B36" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="26" t="s">
         <v>253</v>
       </c>
       <c r="D36" s="24" t="s">
@@ -2874,9 +2839,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32:D36"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2913,7 +2878,7 @@
         <v>339</v>
       </c>
       <c r="D2" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2928,7 +2893,7 @@
         <v>339</v>
       </c>
       <c r="D3" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2943,7 +2908,7 @@
         <v>339</v>
       </c>
       <c r="D4" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2958,7 +2923,7 @@
         <v>339</v>
       </c>
       <c r="D5" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2973,7 +2938,7 @@
         <v>339</v>
       </c>
       <c r="D6" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2988,7 +2953,7 @@
         <v>339</v>
       </c>
       <c r="D7" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3003,7 +2968,7 @@
         <v>339</v>
       </c>
       <c r="D8" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3018,7 +2983,7 @@
         <v>339</v>
       </c>
       <c r="D9" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3033,7 +2998,7 @@
         <v>339</v>
       </c>
       <c r="D10" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3048,7 +3013,7 @@
         <v>339</v>
       </c>
       <c r="D11" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3063,7 +3028,7 @@
         <v>339</v>
       </c>
       <c r="D12" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3078,7 +3043,7 @@
         <v>339</v>
       </c>
       <c r="D13" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3093,7 +3058,7 @@
         <v>339</v>
       </c>
       <c r="D14" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3108,7 +3073,7 @@
         <v>339</v>
       </c>
       <c r="D15" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3123,7 +3088,7 @@
         <v>339</v>
       </c>
       <c r="D16" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3138,7 +3103,7 @@
         <v>339</v>
       </c>
       <c r="D17" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3153,7 +3118,7 @@
         <v>339</v>
       </c>
       <c r="D18" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3168,7 +3133,7 @@
         <v>339</v>
       </c>
       <c r="D19" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3183,7 +3148,7 @@
         <v>339</v>
       </c>
       <c r="D20" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3198,7 +3163,7 @@
         <v>339</v>
       </c>
       <c r="D21" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3213,7 +3178,7 @@
         <v>339</v>
       </c>
       <c r="D22" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3228,7 +3193,7 @@
         <v>339</v>
       </c>
       <c r="D23" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3243,7 +3208,7 @@
         <v>339</v>
       </c>
       <c r="D24" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3258,7 +3223,7 @@
         <v>339</v>
       </c>
       <c r="D25" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3273,7 +3238,7 @@
         <v>339</v>
       </c>
       <c r="D26" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3288,7 +3253,7 @@
         <v>339</v>
       </c>
       <c r="D27" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3303,7 +3268,7 @@
         <v>339</v>
       </c>
       <c r="D28" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3318,7 +3283,7 @@
         <v>339</v>
       </c>
       <c r="D29" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3333,7 +3298,7 @@
         <v>339</v>
       </c>
       <c r="D30" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3348,7 +3313,7 @@
         <v>339</v>
       </c>
       <c r="D31" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3363,67 +3328,67 @@
         <v>339</v>
       </c>
       <c r="D32" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="str">
+      <c r="A33" t="str">
         <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B33" s="37" t="s">
-        <v>354</v>
+      <c r="B33" s="10" t="s">
+        <v>353</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>339</v>
       </c>
       <c r="D33" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="36" t="str">
+      <c r="A34" t="str">
         <f>IF(ISNA(VLOOKUP(B34,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B34" s="37" t="s">
-        <v>351</v>
+      <c r="B34" s="10" t="s">
+        <v>350</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>339</v>
       </c>
       <c r="D34" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="str">
+      <c r="A35" t="str">
         <f>IF(ISNA(VLOOKUP(B35,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B35" s="37" t="s">
-        <v>348</v>
+      <c r="B35" s="10" t="s">
+        <v>347</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>339</v>
       </c>
       <c r="D35" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="str">
+      <c r="A36" t="str">
         <f>IF(ISNA(VLOOKUP(B36,Definitions!B$2:B$1825,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B36" s="37" t="s">
-        <v>349</v>
+      <c r="B36" s="10" t="s">
+        <v>348</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>339</v>
       </c>
       <c r="D36" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update MWD properties excel file
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/mwd_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CE3DF4-7A8B-904A-A38A-9C50AC5B5F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D922F2CB-9668-8B40-9878-FE0AF68C6936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="5040" windowWidth="42140" windowHeight="19460" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10820" yWindow="5040" windowWidth="42140" windowHeight="19460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="384">
   <si>
     <t>Description</t>
   </si>
@@ -699,9 +699,6 @@
     <t>volume per time per volume</t>
   </si>
   <si>
-    <t>unitless</t>
-  </si>
-  <si>
     <t>density or unit weight</t>
   </si>
   <si>
@@ -999,9 +996,6 @@
     <t>Calibration flag</t>
   </si>
   <si>
-    <t>Torque Tach (%)</t>
-  </si>
-  <si>
     <t>Cutting tool rotational speed</t>
   </si>
   <si>
@@ -1186,6 +1180,15 @@
   </si>
   <si>
     <t>ancestor::diggs:measurement//diggs:procedure/diggs:MWDProcedure</t>
+  </si>
+  <si>
+    <t>Hydraulic fluid flow rate</t>
+  </si>
+  <si>
+    <t>Rate of flow of the rig hydraulic fluid.</t>
+  </si>
+  <si>
+    <t>Torque Tach</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1346,6 +1349,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1361,7 +1373,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1434,6 +1446,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1716,10 +1746,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H39" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:H39" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H37">
-    <sortCondition ref="C1:C37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H40" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:H40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H38">
+    <sortCondition ref="C1:C38"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="12">
@@ -1745,7 +1775,7 @@
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="3">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="1"/>
@@ -1756,10 +1786,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table6" displayName="Table6" ref="A1:C188" totalsRowShown="0">
-  <autoFilter ref="A1:C188" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C187">
-    <sortCondition ref="C1:C187"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table6" displayName="Table6" ref="A1:C187" totalsRowShown="0">
+  <autoFilter ref="A1:C187" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C186">
+    <sortCondition ref="C1:C186"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DataType"/>
@@ -2058,7 +2088,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>14</v>
@@ -2073,21 +2103,21 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2102,10 +2132,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2126,7 +2156,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>8</v>
@@ -2138,13 +2168,13 @@
         <v>165</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="136" x14ac:dyDescent="0.2">
@@ -2153,25 +2183,22 @@
         <v/>
       </c>
       <c r="B2" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>337</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>339</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2180,19 +2207,16 @@
         <v/>
       </c>
       <c r="B3" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>174</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2201,13 +2225,13 @@
         <v/>
       </c>
       <c r="B4" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>1</v>
@@ -2222,13 +2246,13 @@
         <v/>
       </c>
       <c r="B5" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>1</v>
@@ -2244,13 +2268,13 @@
         <v/>
       </c>
       <c r="B6" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>289</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>321</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>290</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>1</v>
@@ -2265,13 +2289,13 @@
         <v/>
       </c>
       <c r="B7" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>1</v>
@@ -2280,10 +2304,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="170" x14ac:dyDescent="0.2">
@@ -2292,25 +2316,22 @@
         <v/>
       </c>
       <c r="B8" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>342</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>344</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="G8" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>367</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2319,13 +2340,13 @@
         <v/>
       </c>
       <c r="B9" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>1</v>
@@ -2340,13 +2361,13 @@
         <v/>
       </c>
       <c r="B10" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>1</v>
@@ -2361,13 +2382,13 @@
         <v/>
       </c>
       <c r="B11" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>1</v>
@@ -2382,13 +2403,13 @@
         <v/>
       </c>
       <c r="B12" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>1</v>
@@ -2403,19 +2424,16 @@
         <v/>
       </c>
       <c r="B13" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>294</v>
-      </c>
       <c r="D13" s="22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>180</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>220</v>
       </c>
       <c r="G13" s="19"/>
     </row>
@@ -2425,13 +2443,13 @@
         <v/>
       </c>
       <c r="B14" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>329</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>331</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>1</v>
@@ -2447,25 +2465,22 @@
         <v/>
       </c>
       <c r="B15" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="G15" s="19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -2474,13 +2489,13 @@
         <v/>
       </c>
       <c r="B16" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>326</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>328</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>1</v>
@@ -2496,13 +2511,13 @@
         <v/>
       </c>
       <c r="B17" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>1</v>
@@ -2517,13 +2532,13 @@
         <v/>
       </c>
       <c r="B18" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>1</v>
@@ -2533,259 +2548,252 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2848,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="A19" s="30" t="str">
+        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B2857,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B19" t="s">
+        <v>261</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="E19" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="F19" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="35"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2849,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B2848,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B20" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>311</v>
+        <v>296</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>309</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2854,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B2849,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B21" s="15" t="s">
-        <v>379</v>
+        <v>257</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>286</v>
+        <v>240</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>310</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2853,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B2854,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B22" s="15" t="s">
-        <v>25</v>
+        <v>377</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>348</v>
+        <v>285</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="str">
+        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2853,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B2872,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>323</v>
-      </c>
       <c r="C23" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>325</v>
+        <v>379</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>346</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="19"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>324</v>
+        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B2872,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>321</v>
       </c>
       <c r="C24" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="str">
+        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="D25" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>317</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="E25" s="17" t="s">
         <v>174</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B2852,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B2852,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B26" s="15" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B2842,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B27" s="15" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>359</v>
+        <v>235</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>312</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2843,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B28" s="15" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>288</v>
+        <v>247</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>357</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B2843,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B29" s="15" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>335</v>
+        <v>297</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>365</v>
+        <v>287</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B2874,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B30" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>247</v>
+        <v>332</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>333</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>363</v>
@@ -2794,213 +2802,231 @@
         <v>1</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>10</v>
+        <v>334</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="H30" s="27" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B2873,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B31" s="15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>245</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>355</v>
+        <v>246</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>361</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="G31" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="str">
+        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="H31" s="27" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B2878,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>350</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>314</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="19"/>
+      <c r="G32" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B2840,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B2878,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B33" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>351</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>111</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B2879,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B2840,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B34" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>320</v>
+        <v>249</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>233</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="E34" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="E34" s="21" t="s">
         <v>1</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="19"/>
-    </row>
-    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B2850,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B2879,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B35" s="15" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>299</v>
+        <v>383</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>295</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>84</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G35" s="19"/>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B2850,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B36" s="15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>302</v>
+        <v>331</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>352</v>
+        <v>298</v>
       </c>
       <c r="E36" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B2877,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B37" s="15" t="s">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>350</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B2876,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B2877,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B38" s="15" t="s">
-        <v>361</v>
+        <v>266</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>362</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>375</v>
+        <v>248</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>305</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F38" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="str">
+        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B2876,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="19"/>
-    </row>
-    <row r="39" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B2877,1,FALSE)),"Not used","")</f>
-        <v/>
-      </c>
-      <c r="B39" s="15" t="s">
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="str">
+        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B2877,1,FALSE)),"Not used","")</f>
+        <v/>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="D40" s="22" t="s">
         <v>376</v>
       </c>
-      <c r="C39" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>378</v>
-      </c>
-      <c r="E39" s="17" t="s">
+      <c r="E40" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="19"/>
+      <c r="G40" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -3009,8 +3035,8 @@
     <hyperlink ref="H7" r:id="rId2" xr:uid="{19D7D6E5-5ACE-324A-8460-A6F4DDD4E28B}"/>
     <hyperlink ref="H8" r:id="rId3" xr:uid="{57F0ED7A-11F4-D240-AD82-9CE55AE72124}"/>
     <hyperlink ref="H15" r:id="rId4" xr:uid="{8D50C3BF-C589-C14D-B41C-E99AE03A2CDC}"/>
-    <hyperlink ref="H30" r:id="rId5" xr:uid="{FC3D442E-4CC0-0847-A941-C36DD2CE39AF}"/>
-    <hyperlink ref="H31" r:id="rId6" xr:uid="{0FF5AB1B-449D-8843-B572-B81E096359CD}"/>
+    <hyperlink ref="H31" r:id="rId5" xr:uid="{FC3D442E-4CC0-0847-A941-C36DD2CE39AF}"/>
+    <hyperlink ref="H32" r:id="rId6" xr:uid="{0FF5AB1B-449D-8843-B572-B81E096359CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -3022,15 +3048,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E8BE39A-6790-4C87-932D-CBC46A1C9925}">
           <x14:formula1>
-            <xm:f>Lists!$C$2:$C$187</xm:f>
+            <xm:f>Lists!$C$2:$C$186</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>Lists!$C$2:$C$178</xm:f>
+            <xm:f>Lists!$C$2:$C$177</xm:f>
           </x14:formula1>
-          <xm:sqref>F16:F29</xm:sqref>
+          <xm:sqref>F16:F30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3043,9 +3069,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3061,598 +3087,598 @@
         <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B4,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B5,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D8" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B9,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D11" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D12" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B15,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
-        <v>Not listed</v>
+        <f>IF(ISNA(VLOOKUP(B16,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
+        <v/>
       </c>
       <c r="B16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D16" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D17" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B18,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D18" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D20" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D21" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B22" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D22" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B23,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B23" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B24,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B24" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D24" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B25,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B25" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D25" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B26,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B26" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D26" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B27,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B27" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D27" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B28,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B28" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D28" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B29,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B29" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D29" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B30,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B30" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B31" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B32" s="10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D32" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B33,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B33" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D33" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B34,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B34" s="10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D34" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B35,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B35" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D35" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B36,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B36" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D36" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B37,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B37" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D37" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B38,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B38" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D38" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B39,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B39" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D39" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,Definitions!B$2:B$1822,1,FALSE)),"Not listed","")</f>
+        <f>IF(ISNA(VLOOKUP(B40,Definitions!B$2:B$1823,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
       <c r="B40" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D40" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -3670,10 +3696,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D188"/>
+  <dimension ref="A1:D187"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView topLeftCell="A161" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168:XFD168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3687,10 +3713,10 @@
         <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3855,7 +3881,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C20" t="s">
         <v>200</v>
@@ -3930,7 +3956,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D28" s="7"/>
     </row>
@@ -3996,7 +4022,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C36" t="s">
         <v>49</v>
@@ -4653,7 +4679,7 @@
     </row>
     <row r="145" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C145" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D145" s="7"/>
     </row>
@@ -4791,132 +4817,126 @@
     </row>
     <row r="168" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C168" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D168" s="7"/>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C169" t="s">
-        <v>212</v>
+        <v>155</v>
       </c>
       <c r="D169" s="7"/>
     </row>
     <row r="170" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C170" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D170" s="7"/>
     </row>
     <row r="171" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C171" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D171" s="7"/>
     </row>
     <row r="172" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C172" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D172" s="7"/>
     </row>
     <row r="173" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C173" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D173" s="7"/>
     </row>
     <row r="174" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C174" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D174" s="7"/>
     </row>
     <row r="175" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C175" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D175" s="7"/>
     </row>
     <row r="176" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C176" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D176" s="7"/>
     </row>
     <row r="177" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C177" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
       <c r="D177" s="7"/>
     </row>
     <row r="178" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C178" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D178" s="7"/>
     </row>
     <row r="179" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C179" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D179" s="7"/>
     </row>
     <row r="180" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C180" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D180" s="7"/>
     </row>
     <row r="181" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C181" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D181" s="7"/>
     </row>
     <row r="182" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C182" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D182" s="7"/>
     </row>
     <row r="183" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C183" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D183" s="7"/>
     </row>
     <row r="184" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C184" t="s">
-        <v>219</v>
+        <v>12</v>
       </c>
       <c r="D184" s="7"/>
     </row>
     <row r="185" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C185" t="s">
-        <v>12</v>
-      </c>
-      <c r="D185" s="7"/>
+        <v>163</v>
+      </c>
+      <c r="D185" s="8"/>
     </row>
     <row r="186" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C186" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D186" s="8"/>
     </row>
     <row r="187" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C187" t="s">
-        <v>164</v>
-      </c>
-      <c r="D187" s="8"/>
-    </row>
-    <row r="188" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C188" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F176">
-    <sortCondition ref="F2:F176"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F175">
+    <sortCondition ref="F2:F175"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4938,77 +4958,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>